<commit_message>
Updated available hours -Trevor
</commit_message>
<xml_diff>
--- a/logistics/planning_for_backlog.xlsx
+++ b/logistics/planning_for_backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachaelhogan 1/CS471-S18-BitJunkies/logistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halfl\git\CS471-S18-BitJunkies\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15920" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15915" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deliverables" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -691,21 +691,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.125" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -716,7 +716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -724,7 +724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
@@ -732,17 +732,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -750,7 +750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -758,7 +758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -780,40 +780,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+      <selection activeCell="AV17" sqref="AV17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.1640625" customWidth="1"/>
-    <col min="14" max="14" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.125" customWidth="1"/>
+    <col min="14" max="14" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.6640625" customWidth="1"/>
-    <col min="21" max="21" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="64" width="3.1640625" customWidth="1"/>
+    <col min="19" max="19" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.625" customWidth="1"/>
+    <col min="21" max="21" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="64" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="23" t="s">
         <v>9</v>
@@ -881,7 +881,7 @@
       <c r="BK1" s="23"/>
       <c r="BL1" s="23"/>
     </row>
-    <row r="2" spans="1:64" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -946,7 +946,7 @@
       <c r="BK2" s="24"/>
       <c r="BL2" s="24"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1029,7 @@
       <c r="BK3" s="21"/>
       <c r="BL3" s="22"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.375</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="BK5" s="6"/>
       <c r="BL5" s="10"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -1356,7 +1356,7 @@
       <c r="BK6" s="6"/>
       <c r="BL6" s="10"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1407,8 +1407,8 @@
       <c r="AT7" s="6"/>
       <c r="AU7" s="6"/>
       <c r="AV7" s="6"/>
-      <c r="AW7" s="6"/>
-      <c r="AX7" s="10"/>
+      <c r="AW7" s="16"/>
+      <c r="AX7" s="18"/>
       <c r="AY7" s="9"/>
       <c r="AZ7" s="6"/>
       <c r="BA7" s="6"/>
@@ -1424,7 +1424,7 @@
       <c r="BK7" s="6"/>
       <c r="BL7" s="10"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.4375</v>
       </c>
@@ -1475,8 +1475,8 @@
       <c r="AT8" s="6"/>
       <c r="AU8" s="6"/>
       <c r="AV8" s="6"/>
-      <c r="AW8" s="6"/>
-      <c r="AX8" s="10"/>
+      <c r="AW8" s="16"/>
+      <c r="AX8" s="18"/>
       <c r="AY8" s="9"/>
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
@@ -1492,7 +1492,7 @@
       <c r="BK8" s="6"/>
       <c r="BL8" s="10"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1543,8 +1543,8 @@
       <c r="AT9" s="6"/>
       <c r="AU9" s="6"/>
       <c r="AV9" s="6"/>
-      <c r="AW9" s="6"/>
-      <c r="AX9" s="10"/>
+      <c r="AW9" s="16"/>
+      <c r="AX9" s="18"/>
       <c r="AY9" s="9"/>
       <c r="AZ9" s="6"/>
       <c r="BA9" s="6"/>
@@ -1560,7 +1560,7 @@
       <c r="BK9" s="6"/>
       <c r="BL9" s="10"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.47916666666666702</v>
       </c>
@@ -1611,8 +1611,8 @@
       <c r="AT10" s="6"/>
       <c r="AU10" s="6"/>
       <c r="AV10" s="6"/>
-      <c r="AW10" s="6"/>
-      <c r="AX10" s="10"/>
+      <c r="AW10" s="16"/>
+      <c r="AX10" s="18"/>
       <c r="AY10" s="9"/>
       <c r="AZ10" s="6"/>
       <c r="BA10" s="6"/>
@@ -1628,7 +1628,7 @@
       <c r="BK10" s="6"/>
       <c r="BL10" s="10"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
@@ -1679,8 +1679,8 @@
       <c r="AT11" s="6"/>
       <c r="AU11" s="6"/>
       <c r="AV11" s="6"/>
-      <c r="AW11" s="6"/>
-      <c r="AX11" s="10"/>
+      <c r="AW11" s="16"/>
+      <c r="AX11" s="18"/>
       <c r="AY11" s="9"/>
       <c r="AZ11" s="6"/>
       <c r="BA11" s="6"/>
@@ -1696,7 +1696,7 @@
       <c r="BK11" s="6"/>
       <c r="BL11" s="10"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.52083333333333304</v>
       </c>
@@ -1747,8 +1747,8 @@
       <c r="AT12" s="6"/>
       <c r="AU12" s="6"/>
       <c r="AV12" s="6"/>
-      <c r="AW12" s="6"/>
-      <c r="AX12" s="10"/>
+      <c r="AW12" s="16"/>
+      <c r="AX12" s="18"/>
       <c r="AY12" s="9"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
@@ -1764,7 +1764,7 @@
       <c r="BK12" s="6"/>
       <c r="BL12" s="10"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1815,8 +1815,8 @@
       <c r="AT13" s="6"/>
       <c r="AU13" s="6"/>
       <c r="AV13" s="6"/>
-      <c r="AW13" s="6"/>
-      <c r="AX13" s="10"/>
+      <c r="AW13" s="16"/>
+      <c r="AX13" s="18"/>
       <c r="AY13" s="9"/>
       <c r="AZ13" s="6"/>
       <c r="BA13" s="6"/>
@@ -1832,7 +1832,7 @@
       <c r="BK13" s="6"/>
       <c r="BL13" s="10"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.5625</v>
       </c>
@@ -1883,8 +1883,8 @@
       <c r="AT14" s="6"/>
       <c r="AU14" s="6"/>
       <c r="AV14" s="6"/>
-      <c r="AW14" s="6"/>
-      <c r="AX14" s="10"/>
+      <c r="AW14" s="16"/>
+      <c r="AX14" s="18"/>
       <c r="AY14" s="9"/>
       <c r="AZ14" s="6"/>
       <c r="BA14" s="6"/>
@@ -1900,7 +1900,7 @@
       <c r="BK14" s="6"/>
       <c r="BL14" s="10"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.58333333333333304</v>
       </c>
@@ -1951,8 +1951,8 @@
       <c r="AT15" s="6"/>
       <c r="AU15" s="6"/>
       <c r="AV15" s="6"/>
-      <c r="AW15" s="6"/>
-      <c r="AX15" s="10"/>
+      <c r="AW15" s="16"/>
+      <c r="AX15" s="18"/>
       <c r="AY15" s="9"/>
       <c r="AZ15" s="6"/>
       <c r="BA15" s="6"/>
@@ -1968,7 +1968,7 @@
       <c r="BK15" s="6"/>
       <c r="BL15" s="10"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.60416666666666596</v>
       </c>
@@ -2019,8 +2019,8 @@
       <c r="AT16" s="6"/>
       <c r="AU16" s="6"/>
       <c r="AV16" s="6"/>
-      <c r="AW16" s="6"/>
-      <c r="AX16" s="10"/>
+      <c r="AW16" s="16"/>
+      <c r="AX16" s="18"/>
       <c r="AY16" s="9"/>
       <c r="AZ16" s="6"/>
       <c r="BA16" s="6"/>
@@ -2036,7 +2036,7 @@
       <c r="BK16" s="6"/>
       <c r="BL16" s="10"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -2082,13 +2082,13 @@
       <c r="AO17" s="6"/>
       <c r="AP17" s="6"/>
       <c r="AQ17" s="10"/>
-      <c r="AR17" s="9"/>
+      <c r="AR17" s="14"/>
       <c r="AS17" s="6"/>
-      <c r="AT17" s="6"/>
+      <c r="AT17" s="16"/>
       <c r="AU17" s="6"/>
-      <c r="AV17" s="6"/>
-      <c r="AW17" s="6"/>
-      <c r="AX17" s="10"/>
+      <c r="AV17" s="16"/>
+      <c r="AW17" s="16"/>
+      <c r="AX17" s="18"/>
       <c r="AY17" s="9"/>
       <c r="AZ17" s="6"/>
       <c r="BA17" s="6"/>
@@ -2104,7 +2104,7 @@
       <c r="BK17" s="6"/>
       <c r="BL17" s="10"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.64583333333333304</v>
       </c>
@@ -2150,13 +2150,13 @@
       <c r="AO18" s="6"/>
       <c r="AP18" s="6"/>
       <c r="AQ18" s="10"/>
-      <c r="AR18" s="9"/>
+      <c r="AR18" s="14"/>
       <c r="AS18" s="6"/>
-      <c r="AT18" s="6"/>
+      <c r="AT18" s="16"/>
       <c r="AU18" s="6"/>
-      <c r="AV18" s="6"/>
-      <c r="AW18" s="6"/>
-      <c r="AX18" s="10"/>
+      <c r="AV18" s="16"/>
+      <c r="AW18" s="16"/>
+      <c r="AX18" s="18"/>
       <c r="AY18" s="9"/>
       <c r="AZ18" s="6"/>
       <c r="BA18" s="6"/>
@@ -2172,7 +2172,7 @@
       <c r="BK18" s="6"/>
       <c r="BL18" s="10"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.66666666666666596</v>
       </c>
@@ -2218,13 +2218,13 @@
       <c r="AO19" s="6"/>
       <c r="AP19" s="6"/>
       <c r="AQ19" s="10"/>
-      <c r="AR19" s="9"/>
+      <c r="AR19" s="14"/>
       <c r="AS19" s="6"/>
-      <c r="AT19" s="6"/>
+      <c r="AT19" s="16"/>
       <c r="AU19" s="6"/>
-      <c r="AV19" s="6"/>
-      <c r="AW19" s="6"/>
-      <c r="AX19" s="10"/>
+      <c r="AV19" s="16"/>
+      <c r="AW19" s="16"/>
+      <c r="AX19" s="18"/>
       <c r="AY19" s="9"/>
       <c r="AZ19" s="6"/>
       <c r="BA19" s="6"/>
@@ -2240,7 +2240,7 @@
       <c r="BK19" s="6"/>
       <c r="BL19" s="10"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.6875</v>
       </c>
@@ -2286,13 +2286,13 @@
       <c r="AO20" s="6"/>
       <c r="AP20" s="6"/>
       <c r="AQ20" s="10"/>
-      <c r="AR20" s="9"/>
+      <c r="AR20" s="14"/>
       <c r="AS20" s="6"/>
-      <c r="AT20" s="6"/>
+      <c r="AT20" s="16"/>
       <c r="AU20" s="6"/>
-      <c r="AV20" s="6"/>
-      <c r="AW20" s="6"/>
-      <c r="AX20" s="10"/>
+      <c r="AV20" s="16"/>
+      <c r="AW20" s="16"/>
+      <c r="AX20" s="18"/>
       <c r="AY20" s="9"/>
       <c r="AZ20" s="6"/>
       <c r="BA20" s="6"/>
@@ -2308,7 +2308,7 @@
       <c r="BK20" s="6"/>
       <c r="BL20" s="10"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.70833333333333304</v>
       </c>
@@ -2354,13 +2354,13 @@
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
       <c r="AQ21" s="10"/>
-      <c r="AR21" s="9"/>
+      <c r="AR21" s="14"/>
       <c r="AS21" s="6"/>
-      <c r="AT21" s="6"/>
+      <c r="AT21" s="16"/>
       <c r="AU21" s="6"/>
-      <c r="AV21" s="6"/>
-      <c r="AW21" s="6"/>
-      <c r="AX21" s="10"/>
+      <c r="AV21" s="16"/>
+      <c r="AW21" s="16"/>
+      <c r="AX21" s="18"/>
       <c r="AY21" s="9"/>
       <c r="AZ21" s="6"/>
       <c r="BA21" s="6"/>
@@ -2376,7 +2376,7 @@
       <c r="BK21" s="6"/>
       <c r="BL21" s="10"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.72916666666666596</v>
       </c>
@@ -2422,13 +2422,13 @@
       <c r="AO22" s="6"/>
       <c r="AP22" s="6"/>
       <c r="AQ22" s="10"/>
-      <c r="AR22" s="9"/>
+      <c r="AR22" s="14"/>
       <c r="AS22" s="6"/>
-      <c r="AT22" s="6"/>
+      <c r="AT22" s="16"/>
       <c r="AU22" s="6"/>
-      <c r="AV22" s="6"/>
-      <c r="AW22" s="6"/>
-      <c r="AX22" s="10"/>
+      <c r="AV22" s="16"/>
+      <c r="AW22" s="16"/>
+      <c r="AX22" s="18"/>
       <c r="AY22" s="9"/>
       <c r="AZ22" s="6"/>
       <c r="BA22" s="6"/>
@@ -2444,7 +2444,7 @@
       <c r="BK22" s="6"/>
       <c r="BL22" s="10"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.75</v>
       </c>
@@ -2490,13 +2490,13 @@
       <c r="AO23" s="6"/>
       <c r="AP23" s="6"/>
       <c r="AQ23" s="10"/>
-      <c r="AR23" s="9"/>
-      <c r="AS23" s="6"/>
-      <c r="AT23" s="6"/>
-      <c r="AU23" s="6"/>
-      <c r="AV23" s="6"/>
-      <c r="AW23" s="6"/>
-      <c r="AX23" s="10"/>
+      <c r="AR23" s="14"/>
+      <c r="AS23" s="16"/>
+      <c r="AT23" s="16"/>
+      <c r="AU23" s="16"/>
+      <c r="AV23" s="16"/>
+      <c r="AW23" s="16"/>
+      <c r="AX23" s="18"/>
       <c r="AY23" s="9"/>
       <c r="AZ23" s="6"/>
       <c r="BA23" s="6"/>
@@ -2512,7 +2512,7 @@
       <c r="BK23" s="6"/>
       <c r="BL23" s="10"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.77083333333333304</v>
       </c>
@@ -2558,13 +2558,13 @@
       <c r="AO24" s="6"/>
       <c r="AP24" s="6"/>
       <c r="AQ24" s="10"/>
-      <c r="AR24" s="9"/>
-      <c r="AS24" s="6"/>
-      <c r="AT24" s="6"/>
-      <c r="AU24" s="6"/>
-      <c r="AV24" s="6"/>
-      <c r="AW24" s="6"/>
-      <c r="AX24" s="10"/>
+      <c r="AR24" s="14"/>
+      <c r="AS24" s="16"/>
+      <c r="AT24" s="16"/>
+      <c r="AU24" s="16"/>
+      <c r="AV24" s="16"/>
+      <c r="AW24" s="16"/>
+      <c r="AX24" s="18"/>
       <c r="AY24" s="9"/>
       <c r="AZ24" s="6"/>
       <c r="BA24" s="6"/>
@@ -2580,7 +2580,7 @@
       <c r="BK24" s="6"/>
       <c r="BL24" s="10"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.79166666666666596</v>
       </c>
@@ -2626,12 +2626,12 @@
       <c r="AO25" s="6"/>
       <c r="AP25" s="6"/>
       <c r="AQ25" s="10"/>
-      <c r="AR25" s="9"/>
-      <c r="AS25" s="6"/>
-      <c r="AT25" s="6"/>
-      <c r="AU25" s="6"/>
-      <c r="AV25" s="6"/>
-      <c r="AW25" s="6"/>
+      <c r="AR25" s="14"/>
+      <c r="AS25" s="16"/>
+      <c r="AT25" s="16"/>
+      <c r="AU25" s="16"/>
+      <c r="AV25" s="16"/>
+      <c r="AW25" s="16"/>
       <c r="AX25" s="10"/>
       <c r="AY25" s="9"/>
       <c r="AZ25" s="6"/>
@@ -2648,7 +2648,7 @@
       <c r="BK25" s="6"/>
       <c r="BL25" s="10"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0.8125</v>
       </c>
@@ -2694,12 +2694,12 @@
       <c r="AO26" s="6"/>
       <c r="AP26" s="6"/>
       <c r="AQ26" s="10"/>
-      <c r="AR26" s="9"/>
-      <c r="AS26" s="6"/>
-      <c r="AT26" s="6"/>
-      <c r="AU26" s="6"/>
-      <c r="AV26" s="6"/>
-      <c r="AW26" s="6"/>
+      <c r="AR26" s="14"/>
+      <c r="AS26" s="16"/>
+      <c r="AT26" s="16"/>
+      <c r="AU26" s="16"/>
+      <c r="AV26" s="16"/>
+      <c r="AW26" s="16"/>
       <c r="AX26" s="10"/>
       <c r="AY26" s="9"/>
       <c r="AZ26" s="6"/>
@@ -2716,7 +2716,7 @@
       <c r="BK26" s="6"/>
       <c r="BL26" s="10"/>
     </row>
-    <row r="27" spans="1:64" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>0.83333333333333304</v>
       </c>
@@ -2762,12 +2762,12 @@
       <c r="AO27" s="12"/>
       <c r="AP27" s="12"/>
       <c r="AQ27" s="13"/>
-      <c r="AR27" s="11"/>
-      <c r="AS27" s="12"/>
-      <c r="AT27" s="12"/>
-      <c r="AU27" s="12"/>
-      <c r="AV27" s="12"/>
-      <c r="AW27" s="12"/>
+      <c r="AR27" s="15"/>
+      <c r="AS27" s="17"/>
+      <c r="AT27" s="17"/>
+      <c r="AU27" s="17"/>
+      <c r="AV27" s="17"/>
+      <c r="AW27" s="17"/>
       <c r="AX27" s="13"/>
       <c r="AY27" s="11"/>
       <c r="AZ27" s="12"/>

</xml_diff>

<commit_message>
Added my availability to the schedule
</commit_message>
<xml_diff>
--- a/logistics/planning_for_backlog.xlsx
+++ b/logistics/planning_for_backlog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halfl\git\CS471-S18-BitJunkies\logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K1ASER\git\CS471-S18-BitJunkies\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15915" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="15912" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Deliverables" sheetId="1" r:id="rId1"/>
@@ -131,10 +131,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +183,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -337,17 +350,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -378,8 +392,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -691,21 +710,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -716,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -724,7 +743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
@@ -732,17 +751,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -750,7 +769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -758,7 +777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -766,7 +785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -780,40 +799,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="AV17" sqref="AV17"/>
+      <selection activeCell="BF20" sqref="BF20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.8984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.125" customWidth="1"/>
-    <col min="14" max="14" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.09765625" customWidth="1"/>
+    <col min="14" max="14" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.8984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.625" customWidth="1"/>
-    <col min="21" max="21" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="64" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.59765625" customWidth="1"/>
+    <col min="21" max="21" width="3.8984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="64" width="3.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="23" t="s">
         <v>9</v>
@@ -881,7 +900,7 @@
       <c r="BK1" s="23"/>
       <c r="BL1" s="23"/>
     </row>
-    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -946,7 +965,7 @@
       <c r="BK2" s="24"/>
       <c r="BL2" s="24"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1048,7 @@
       <c r="BK3" s="21"/>
       <c r="BL3" s="22"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1220,7 +1239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.375</v>
       </c>
@@ -1273,11 +1292,11 @@
       <c r="AV5" s="6"/>
       <c r="AW5" s="6"/>
       <c r="AX5" s="10"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" s="6"/>
-      <c r="BA5" s="6"/>
-      <c r="BB5" s="6"/>
-      <c r="BC5" s="6"/>
+      <c r="AY5" s="16"/>
+      <c r="AZ5" s="26"/>
+      <c r="BA5" s="26"/>
+      <c r="BB5" s="26"/>
+      <c r="BC5" s="26"/>
       <c r="BD5" s="6"/>
       <c r="BE5" s="10"/>
       <c r="BF5" s="9"/>
@@ -1288,7 +1307,7 @@
       <c r="BK5" s="6"/>
       <c r="BL5" s="10"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -1341,11 +1360,11 @@
       <c r="AV6" s="6"/>
       <c r="AW6" s="6"/>
       <c r="AX6" s="10"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="6"/>
-      <c r="BA6" s="6"/>
-      <c r="BB6" s="6"/>
-      <c r="BC6" s="6"/>
+      <c r="AY6" s="16"/>
+      <c r="AZ6" s="26"/>
+      <c r="BA6" s="26"/>
+      <c r="BB6" s="26"/>
+      <c r="BC6" s="26"/>
       <c r="BD6" s="6"/>
       <c r="BE6" s="10"/>
       <c r="BF6" s="9"/>
@@ -1356,7 +1375,7 @@
       <c r="BK6" s="6"/>
       <c r="BL6" s="10"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1409,11 +1428,11 @@
       <c r="AV7" s="6"/>
       <c r="AW7" s="16"/>
       <c r="AX7" s="18"/>
-      <c r="AY7" s="9"/>
-      <c r="AZ7" s="6"/>
-      <c r="BA7" s="6"/>
-      <c r="BB7" s="6"/>
-      <c r="BC7" s="6"/>
+      <c r="AY7" s="16"/>
+      <c r="AZ7" s="26"/>
+      <c r="BA7" s="26"/>
+      <c r="BB7" s="26"/>
+      <c r="BC7" s="26"/>
       <c r="BD7" s="6"/>
       <c r="BE7" s="10"/>
       <c r="BF7" s="9"/>
@@ -1424,7 +1443,7 @@
       <c r="BK7" s="6"/>
       <c r="BL7" s="10"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.4375</v>
       </c>
@@ -1477,11 +1496,11 @@
       <c r="AV8" s="6"/>
       <c r="AW8" s="16"/>
       <c r="AX8" s="18"/>
-      <c r="AY8" s="9"/>
-      <c r="AZ8" s="6"/>
-      <c r="BA8" s="6"/>
-      <c r="BB8" s="6"/>
-      <c r="BC8" s="6"/>
+      <c r="AY8" s="16"/>
+      <c r="AZ8" s="26"/>
+      <c r="BA8" s="26"/>
+      <c r="BB8" s="26"/>
+      <c r="BC8" s="26"/>
       <c r="BD8" s="6"/>
       <c r="BE8" s="10"/>
       <c r="BF8" s="9"/>
@@ -1492,7 +1511,7 @@
       <c r="BK8" s="6"/>
       <c r="BL8" s="10"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1545,11 +1564,11 @@
       <c r="AV9" s="6"/>
       <c r="AW9" s="16"/>
       <c r="AX9" s="18"/>
-      <c r="AY9" s="9"/>
-      <c r="AZ9" s="6"/>
-      <c r="BA9" s="6"/>
-      <c r="BB9" s="6"/>
-      <c r="BC9" s="6"/>
+      <c r="AY9" s="16"/>
+      <c r="AZ9" s="26"/>
+      <c r="BA9" s="26"/>
+      <c r="BB9" s="26"/>
+      <c r="BC9" s="26"/>
       <c r="BD9" s="6"/>
       <c r="BE9" s="10"/>
       <c r="BF9" s="9"/>
@@ -1560,7 +1579,7 @@
       <c r="BK9" s="6"/>
       <c r="BL9" s="10"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.47916666666666702</v>
       </c>
@@ -1613,11 +1632,11 @@
       <c r="AV10" s="6"/>
       <c r="AW10" s="16"/>
       <c r="AX10" s="18"/>
-      <c r="AY10" s="9"/>
-      <c r="AZ10" s="6"/>
-      <c r="BA10" s="6"/>
-      <c r="BB10" s="6"/>
-      <c r="BC10" s="6"/>
+      <c r="AY10" s="16"/>
+      <c r="AZ10" s="26"/>
+      <c r="BA10" s="26"/>
+      <c r="BB10" s="26"/>
+      <c r="BC10" s="26"/>
       <c r="BD10" s="6"/>
       <c r="BE10" s="10"/>
       <c r="BF10" s="9"/>
@@ -1628,7 +1647,7 @@
       <c r="BK10" s="6"/>
       <c r="BL10" s="10"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
@@ -1682,10 +1701,10 @@
       <c r="AW11" s="16"/>
       <c r="AX11" s="18"/>
       <c r="AY11" s="9"/>
-      <c r="AZ11" s="6"/>
+      <c r="AZ11" s="26"/>
       <c r="BA11" s="6"/>
-      <c r="BB11" s="6"/>
-      <c r="BC11" s="6"/>
+      <c r="BB11" s="26"/>
+      <c r="BC11" s="26"/>
       <c r="BD11" s="6"/>
       <c r="BE11" s="10"/>
       <c r="BF11" s="9"/>
@@ -1696,7 +1715,7 @@
       <c r="BK11" s="6"/>
       <c r="BL11" s="10"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.52083333333333304</v>
       </c>
@@ -1750,10 +1769,10 @@
       <c r="AW12" s="16"/>
       <c r="AX12" s="18"/>
       <c r="AY12" s="9"/>
-      <c r="AZ12" s="6"/>
+      <c r="AZ12" s="26"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="6"/>
-      <c r="BC12" s="6"/>
+      <c r="BB12" s="26"/>
+      <c r="BC12" s="26"/>
       <c r="BD12" s="6"/>
       <c r="BE12" s="10"/>
       <c r="BF12" s="9"/>
@@ -1764,7 +1783,7 @@
       <c r="BK12" s="6"/>
       <c r="BL12" s="10"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1818,10 +1837,10 @@
       <c r="AW13" s="16"/>
       <c r="AX13" s="18"/>
       <c r="AY13" s="9"/>
-      <c r="AZ13" s="6"/>
+      <c r="AZ13" s="26"/>
       <c r="BA13" s="6"/>
-      <c r="BB13" s="6"/>
-      <c r="BC13" s="6"/>
+      <c r="BB13" s="26"/>
+      <c r="BC13" s="26"/>
       <c r="BD13" s="6"/>
       <c r="BE13" s="10"/>
       <c r="BF13" s="9"/>
@@ -1832,7 +1851,7 @@
       <c r="BK13" s="6"/>
       <c r="BL13" s="10"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.5625</v>
       </c>
@@ -1886,10 +1905,10 @@
       <c r="AW14" s="16"/>
       <c r="AX14" s="18"/>
       <c r="AY14" s="9"/>
-      <c r="AZ14" s="6"/>
+      <c r="AZ14" s="26"/>
       <c r="BA14" s="6"/>
-      <c r="BB14" s="6"/>
-      <c r="BC14" s="6"/>
+      <c r="BB14" s="26"/>
+      <c r="BC14" s="26"/>
       <c r="BD14" s="6"/>
       <c r="BE14" s="10"/>
       <c r="BF14" s="9"/>
@@ -1900,7 +1919,7 @@
       <c r="BK14" s="6"/>
       <c r="BL14" s="10"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.58333333333333304</v>
       </c>
@@ -1954,10 +1973,10 @@
       <c r="AW15" s="16"/>
       <c r="AX15" s="18"/>
       <c r="AY15" s="9"/>
-      <c r="AZ15" s="6"/>
+      <c r="AZ15" s="26"/>
       <c r="BA15" s="6"/>
-      <c r="BB15" s="6"/>
-      <c r="BC15" s="6"/>
+      <c r="BB15" s="26"/>
+      <c r="BC15" s="26"/>
       <c r="BD15" s="6"/>
       <c r="BE15" s="10"/>
       <c r="BF15" s="9"/>
@@ -1968,7 +1987,7 @@
       <c r="BK15" s="6"/>
       <c r="BL15" s="10"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.60416666666666596</v>
       </c>
@@ -2022,10 +2041,10 @@
       <c r="AW16" s="16"/>
       <c r="AX16" s="18"/>
       <c r="AY16" s="9"/>
-      <c r="AZ16" s="6"/>
+      <c r="AZ16" s="26"/>
       <c r="BA16" s="6"/>
-      <c r="BB16" s="6"/>
-      <c r="BC16" s="6"/>
+      <c r="BB16" s="26"/>
+      <c r="BC16" s="26"/>
       <c r="BD16" s="6"/>
       <c r="BE16" s="10"/>
       <c r="BF16" s="9"/>
@@ -2036,7 +2055,7 @@
       <c r="BK16" s="6"/>
       <c r="BL16" s="10"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -2089,11 +2108,11 @@
       <c r="AV17" s="16"/>
       <c r="AW17" s="16"/>
       <c r="AX17" s="18"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="6"/>
-      <c r="BA17" s="6"/>
-      <c r="BB17" s="6"/>
-      <c r="BC17" s="6"/>
+      <c r="AY17" s="25"/>
+      <c r="AZ17" s="26"/>
+      <c r="BA17" s="26"/>
+      <c r="BB17" s="26"/>
+      <c r="BC17" s="26"/>
       <c r="BD17" s="6"/>
       <c r="BE17" s="10"/>
       <c r="BF17" s="9"/>
@@ -2104,7 +2123,7 @@
       <c r="BK17" s="6"/>
       <c r="BL17" s="10"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0.64583333333333304</v>
       </c>
@@ -2157,11 +2176,11 @@
       <c r="AV18" s="16"/>
       <c r="AW18" s="16"/>
       <c r="AX18" s="18"/>
-      <c r="AY18" s="9"/>
-      <c r="AZ18" s="6"/>
-      <c r="BA18" s="6"/>
-      <c r="BB18" s="6"/>
-      <c r="BC18" s="6"/>
+      <c r="AY18" s="25"/>
+      <c r="AZ18" s="26"/>
+      <c r="BA18" s="26"/>
+      <c r="BB18" s="26"/>
+      <c r="BC18" s="26"/>
       <c r="BD18" s="6"/>
       <c r="BE18" s="10"/>
       <c r="BF18" s="9"/>
@@ -2172,7 +2191,7 @@
       <c r="BK18" s="6"/>
       <c r="BL18" s="10"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.66666666666666596</v>
       </c>
@@ -2225,11 +2244,11 @@
       <c r="AV19" s="16"/>
       <c r="AW19" s="16"/>
       <c r="AX19" s="18"/>
-      <c r="AY19" s="9"/>
-      <c r="AZ19" s="6"/>
-      <c r="BA19" s="6"/>
-      <c r="BB19" s="6"/>
-      <c r="BC19" s="6"/>
+      <c r="AY19" s="25"/>
+      <c r="AZ19" s="26"/>
+      <c r="BA19" s="26"/>
+      <c r="BB19" s="26"/>
+      <c r="BC19" s="26"/>
       <c r="BD19" s="6"/>
       <c r="BE19" s="10"/>
       <c r="BF19" s="9"/>
@@ -2240,7 +2259,7 @@
       <c r="BK19" s="6"/>
       <c r="BL19" s="10"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0.6875</v>
       </c>
@@ -2293,11 +2312,11 @@
       <c r="AV20" s="16"/>
       <c r="AW20" s="16"/>
       <c r="AX20" s="18"/>
-      <c r="AY20" s="9"/>
-      <c r="AZ20" s="6"/>
-      <c r="BA20" s="6"/>
-      <c r="BB20" s="6"/>
-      <c r="BC20" s="6"/>
+      <c r="AY20" s="25"/>
+      <c r="AZ20" s="26"/>
+      <c r="BA20" s="26"/>
+      <c r="BB20" s="26"/>
+      <c r="BC20" s="26"/>
       <c r="BD20" s="6"/>
       <c r="BE20" s="10"/>
       <c r="BF20" s="9"/>
@@ -2308,7 +2327,7 @@
       <c r="BK20" s="6"/>
       <c r="BL20" s="10"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.70833333333333304</v>
       </c>
@@ -2361,11 +2380,11 @@
       <c r="AV21" s="16"/>
       <c r="AW21" s="16"/>
       <c r="AX21" s="18"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="6"/>
-      <c r="BA21" s="6"/>
-      <c r="BB21" s="6"/>
-      <c r="BC21" s="6"/>
+      <c r="AY21" s="25"/>
+      <c r="AZ21" s="26"/>
+      <c r="BA21" s="26"/>
+      <c r="BB21" s="26"/>
+      <c r="BC21" s="26"/>
       <c r="BD21" s="6"/>
       <c r="BE21" s="10"/>
       <c r="BF21" s="9"/>
@@ -2376,7 +2395,7 @@
       <c r="BK21" s="6"/>
       <c r="BL21" s="10"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>0.72916666666666596</v>
       </c>
@@ -2429,11 +2448,11 @@
       <c r="AV22" s="16"/>
       <c r="AW22" s="16"/>
       <c r="AX22" s="18"/>
-      <c r="AY22" s="9"/>
-      <c r="AZ22" s="6"/>
-      <c r="BA22" s="6"/>
-      <c r="BB22" s="6"/>
-      <c r="BC22" s="6"/>
+      <c r="AY22" s="25"/>
+      <c r="AZ22" s="26"/>
+      <c r="BA22" s="26"/>
+      <c r="BB22" s="26"/>
+      <c r="BC22" s="26"/>
       <c r="BD22" s="6"/>
       <c r="BE22" s="10"/>
       <c r="BF22" s="9"/>
@@ -2444,7 +2463,7 @@
       <c r="BK22" s="6"/>
       <c r="BL22" s="10"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.75</v>
       </c>
@@ -2497,11 +2516,11 @@
       <c r="AV23" s="16"/>
       <c r="AW23" s="16"/>
       <c r="AX23" s="18"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="6"/>
-      <c r="BA23" s="6"/>
-      <c r="BB23" s="6"/>
-      <c r="BC23" s="6"/>
+      <c r="AY23" s="25"/>
+      <c r="AZ23" s="26"/>
+      <c r="BA23" s="26"/>
+      <c r="BB23" s="26"/>
+      <c r="BC23" s="26"/>
       <c r="BD23" s="6"/>
       <c r="BE23" s="10"/>
       <c r="BF23" s="9"/>
@@ -2512,7 +2531,7 @@
       <c r="BK23" s="6"/>
       <c r="BL23" s="10"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.77083333333333304</v>
       </c>
@@ -2565,11 +2584,11 @@
       <c r="AV24" s="16"/>
       <c r="AW24" s="16"/>
       <c r="AX24" s="18"/>
-      <c r="AY24" s="9"/>
-      <c r="AZ24" s="6"/>
-      <c r="BA24" s="6"/>
-      <c r="BB24" s="6"/>
-      <c r="BC24" s="6"/>
+      <c r="AY24" s="25"/>
+      <c r="AZ24" s="26"/>
+      <c r="BA24" s="26"/>
+      <c r="BB24" s="26"/>
+      <c r="BC24" s="26"/>
       <c r="BD24" s="6"/>
       <c r="BE24" s="10"/>
       <c r="BF24" s="9"/>
@@ -2580,7 +2599,7 @@
       <c r="BK24" s="6"/>
       <c r="BL24" s="10"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.79166666666666596</v>
       </c>
@@ -2633,11 +2652,11 @@
       <c r="AV25" s="16"/>
       <c r="AW25" s="16"/>
       <c r="AX25" s="10"/>
-      <c r="AY25" s="9"/>
-      <c r="AZ25" s="6"/>
-      <c r="BA25" s="6"/>
-      <c r="BB25" s="6"/>
-      <c r="BC25" s="6"/>
+      <c r="AY25" s="25"/>
+      <c r="AZ25" s="26"/>
+      <c r="BA25" s="26"/>
+      <c r="BB25" s="26"/>
+      <c r="BC25" s="26"/>
       <c r="BD25" s="6"/>
       <c r="BE25" s="10"/>
       <c r="BF25" s="9"/>
@@ -2648,7 +2667,7 @@
       <c r="BK25" s="6"/>
       <c r="BL25" s="10"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>0.8125</v>
       </c>
@@ -2701,11 +2720,11 @@
       <c r="AV26" s="16"/>
       <c r="AW26" s="16"/>
       <c r="AX26" s="10"/>
-      <c r="AY26" s="9"/>
-      <c r="AZ26" s="6"/>
-      <c r="BA26" s="6"/>
-      <c r="BB26" s="6"/>
-      <c r="BC26" s="6"/>
+      <c r="AY26" s="25"/>
+      <c r="AZ26" s="26"/>
+      <c r="BA26" s="26"/>
+      <c r="BB26" s="26"/>
+      <c r="BC26" s="26"/>
       <c r="BD26" s="6"/>
       <c r="BE26" s="10"/>
       <c r="BF26" s="9"/>
@@ -2716,7 +2735,7 @@
       <c r="BK26" s="6"/>
       <c r="BL26" s="10"/>
     </row>
-    <row r="27" spans="1:64" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>0.83333333333333304</v>
       </c>
@@ -2769,11 +2788,11 @@
       <c r="AV27" s="17"/>
       <c r="AW27" s="17"/>
       <c r="AX27" s="13"/>
-      <c r="AY27" s="11"/>
-      <c r="AZ27" s="12"/>
-      <c r="BA27" s="12"/>
-      <c r="BB27" s="12"/>
-      <c r="BC27" s="12"/>
+      <c r="AY27" s="27"/>
+      <c r="AZ27" s="28"/>
+      <c r="BA27" s="28"/>
+      <c r="BB27" s="28"/>
+      <c r="BC27" s="28"/>
       <c r="BD27" s="12"/>
       <c r="BE27" s="13"/>
       <c r="BF27" s="11"/>

</xml_diff>

<commit_message>
updated availability - Nate
</commit_message>
<xml_diff>
--- a/logistics/planning_for_backlog.xlsx
+++ b/logistics/planning_for_backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halfl\git\CS471-S18-BitJunkies\logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\Boise State\Spring 2018\CS471\groupProject\CS471-S18-BitJunkies\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15915" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="15918" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deliverables" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,8 +156,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +183,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -337,10 +349,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -378,8 +391,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="18" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -698,14 +714,14 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="2" max="2" width="30.09765625" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -716,7 +732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -724,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
@@ -732,17 +748,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -750,7 +766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -758,7 +774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -766,7 +782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.6">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -783,37 +799,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="AV17" sqref="AV17"/>
+    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="131" workbookViewId="0">
+      <selection activeCell="AP10" sqref="AP10:AP23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.125" customWidth="1"/>
-    <col min="14" max="14" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.09765625" customWidth="1"/>
+    <col min="14" max="14" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.625" customWidth="1"/>
-    <col min="21" max="21" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="64" width="3.125" customWidth="1"/>
+    <col min="19" max="19" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.59765625" customWidth="1"/>
+    <col min="21" max="21" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.09765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="64" width="3.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A1" s="4"/>
       <c r="B1" s="23" t="s">
         <v>9</v>
@@ -881,7 +897,7 @@
       <c r="BK1" s="23"/>
       <c r="BL1" s="23"/>
     </row>
-    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -946,7 +962,7 @@
       <c r="BK2" s="24"/>
       <c r="BL2" s="24"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.6">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1029,7 +1045,7 @@
       <c r="BK3" s="21"/>
       <c r="BL3" s="22"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.6">
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1220,7 +1236,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A5" s="1">
         <v>0.375</v>
       </c>
@@ -1288,7 +1304,7 @@
       <c r="BK5" s="6"/>
       <c r="BL5" s="10"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A6" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -1356,7 +1372,7 @@
       <c r="BK6" s="6"/>
       <c r="BL6" s="10"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A7" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1424,7 +1440,7 @@
       <c r="BK7" s="6"/>
       <c r="BL7" s="10"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A8" s="1">
         <v>0.4375</v>
       </c>
@@ -1492,7 +1508,7 @@
       <c r="BK8" s="6"/>
       <c r="BL8" s="10"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A9" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1560,7 +1576,7 @@
       <c r="BK9" s="6"/>
       <c r="BL9" s="10"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A10" s="1">
         <v>0.47916666666666702</v>
       </c>
@@ -1604,7 +1620,7 @@
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
       <c r="AO10" s="6"/>
-      <c r="AP10" s="6"/>
+      <c r="AP10" s="25"/>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="9"/>
       <c r="AS10" s="6"/>
@@ -1628,7 +1644,7 @@
       <c r="BK10" s="6"/>
       <c r="BL10" s="10"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
@@ -1672,7 +1688,7 @@
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
       <c r="AO11" s="6"/>
-      <c r="AP11" s="6"/>
+      <c r="AP11" s="25"/>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="9"/>
       <c r="AS11" s="6"/>
@@ -1696,7 +1712,7 @@
       <c r="BK11" s="6"/>
       <c r="BL11" s="10"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A12" s="1">
         <v>0.52083333333333304</v>
       </c>
@@ -1740,7 +1756,7 @@
       <c r="AM12" s="6"/>
       <c r="AN12" s="6"/>
       <c r="AO12" s="6"/>
-      <c r="AP12" s="6"/>
+      <c r="AP12" s="25"/>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="9"/>
       <c r="AS12" s="6"/>
@@ -1764,7 +1780,7 @@
       <c r="BK12" s="6"/>
       <c r="BL12" s="10"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A13" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1808,7 +1824,7 @@
       <c r="AM13" s="6"/>
       <c r="AN13" s="6"/>
       <c r="AO13" s="6"/>
-      <c r="AP13" s="6"/>
+      <c r="AP13" s="25"/>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="9"/>
       <c r="AS13" s="6"/>
@@ -1832,7 +1848,7 @@
       <c r="BK13" s="6"/>
       <c r="BL13" s="10"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A14" s="1">
         <v>0.5625</v>
       </c>
@@ -1876,7 +1892,7 @@
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
       <c r="AO14" s="6"/>
-      <c r="AP14" s="6"/>
+      <c r="AP14" s="25"/>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="9"/>
       <c r="AS14" s="6"/>
@@ -1900,7 +1916,7 @@
       <c r="BK14" s="6"/>
       <c r="BL14" s="10"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A15" s="1">
         <v>0.58333333333333304</v>
       </c>
@@ -1939,12 +1955,12 @@
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="10"/>
-      <c r="AK15" s="9"/>
+      <c r="AK15" s="26"/>
       <c r="AL15" s="6"/>
-      <c r="AM15" s="6"/>
+      <c r="AM15" s="25"/>
       <c r="AN15" s="6"/>
-      <c r="AO15" s="6"/>
-      <c r="AP15" s="6"/>
+      <c r="AO15" s="25"/>
+      <c r="AP15" s="25"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="9"/>
       <c r="AS15" s="6"/>
@@ -1968,7 +1984,7 @@
       <c r="BK15" s="6"/>
       <c r="BL15" s="10"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A16" s="1">
         <v>0.60416666666666596</v>
       </c>
@@ -2007,12 +2023,12 @@
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="10"/>
-      <c r="AK16" s="9"/>
+      <c r="AK16" s="26"/>
       <c r="AL16" s="6"/>
-      <c r="AM16" s="6"/>
+      <c r="AM16" s="25"/>
       <c r="AN16" s="6"/>
-      <c r="AO16" s="6"/>
-      <c r="AP16" s="6"/>
+      <c r="AO16" s="25"/>
+      <c r="AP16" s="25"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="9"/>
       <c r="AS16" s="6"/>
@@ -2036,7 +2052,7 @@
       <c r="BK16" s="6"/>
       <c r="BL16" s="10"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -2075,18 +2091,18 @@
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="10"/>
-      <c r="AK17" s="9"/>
+      <c r="AK17" s="26"/>
       <c r="AL17" s="6"/>
-      <c r="AM17" s="6"/>
+      <c r="AM17" s="25"/>
       <c r="AN17" s="6"/>
-      <c r="AO17" s="6"/>
-      <c r="AP17" s="6"/>
+      <c r="AO17" s="25"/>
+      <c r="AP17" s="25"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="14"/>
       <c r="AS17" s="6"/>
       <c r="AT17" s="16"/>
       <c r="AU17" s="6"/>
-      <c r="AV17" s="16"/>
+      <c r="AV17" s="25"/>
       <c r="AW17" s="16"/>
       <c r="AX17" s="18"/>
       <c r="AY17" s="9"/>
@@ -2104,7 +2120,7 @@
       <c r="BK17" s="6"/>
       <c r="BL17" s="10"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A18" s="1">
         <v>0.64583333333333304</v>
       </c>
@@ -2143,12 +2159,12 @@
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="10"/>
-      <c r="AK18" s="9"/>
+      <c r="AK18" s="26"/>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="6"/>
+      <c r="AM18" s="25"/>
       <c r="AN18" s="6"/>
-      <c r="AO18" s="6"/>
-      <c r="AP18" s="6"/>
+      <c r="AO18" s="25"/>
+      <c r="AP18" s="25"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="14"/>
       <c r="AS18" s="6"/>
@@ -2172,7 +2188,7 @@
       <c r="BK18" s="6"/>
       <c r="BL18" s="10"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A19" s="1">
         <v>0.66666666666666596</v>
       </c>
@@ -2211,12 +2227,12 @@
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="9"/>
+      <c r="AK19" s="26"/>
       <c r="AL19" s="6"/>
-      <c r="AM19" s="6"/>
+      <c r="AM19" s="25"/>
       <c r="AN19" s="6"/>
-      <c r="AO19" s="6"/>
-      <c r="AP19" s="6"/>
+      <c r="AO19" s="25"/>
+      <c r="AP19" s="25"/>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="14"/>
       <c r="AS19" s="6"/>
@@ -2240,7 +2256,7 @@
       <c r="BK19" s="6"/>
       <c r="BL19" s="10"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A20" s="1">
         <v>0.6875</v>
       </c>
@@ -2279,12 +2295,12 @@
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="9"/>
+      <c r="AK20" s="26"/>
       <c r="AL20" s="6"/>
-      <c r="AM20" s="6"/>
+      <c r="AM20" s="25"/>
       <c r="AN20" s="6"/>
-      <c r="AO20" s="6"/>
-      <c r="AP20" s="6"/>
+      <c r="AO20" s="25"/>
+      <c r="AP20" s="25"/>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="14"/>
       <c r="AS20" s="6"/>
@@ -2308,7 +2324,7 @@
       <c r="BK20" s="6"/>
       <c r="BL20" s="10"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A21" s="1">
         <v>0.70833333333333304</v>
       </c>
@@ -2347,12 +2363,12 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="10"/>
-      <c r="AK21" s="9"/>
+      <c r="AK21" s="26"/>
       <c r="AL21" s="6"/>
-      <c r="AM21" s="6"/>
+      <c r="AM21" s="25"/>
       <c r="AN21" s="6"/>
-      <c r="AO21" s="6"/>
-      <c r="AP21" s="6"/>
+      <c r="AO21" s="25"/>
+      <c r="AP21" s="25"/>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="14"/>
       <c r="AS21" s="6"/>
@@ -2376,7 +2392,7 @@
       <c r="BK21" s="6"/>
       <c r="BL21" s="10"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A22" s="1">
         <v>0.72916666666666596</v>
       </c>
@@ -2415,12 +2431,12 @@
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="10"/>
-      <c r="AK22" s="9"/>
+      <c r="AK22" s="26"/>
       <c r="AL22" s="6"/>
-      <c r="AM22" s="6"/>
+      <c r="AM22" s="25"/>
       <c r="AN22" s="6"/>
-      <c r="AO22" s="6"/>
-      <c r="AP22" s="6"/>
+      <c r="AO22" s="25"/>
+      <c r="AP22" s="25"/>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="14"/>
       <c r="AS22" s="6"/>
@@ -2444,7 +2460,7 @@
       <c r="BK22" s="6"/>
       <c r="BL22" s="10"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A23" s="1">
         <v>0.75</v>
       </c>
@@ -2483,12 +2499,12 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="10"/>
-      <c r="AK23" s="9"/>
+      <c r="AK23" s="26"/>
       <c r="AL23" s="6"/>
-      <c r="AM23" s="6"/>
+      <c r="AM23" s="25"/>
       <c r="AN23" s="6"/>
-      <c r="AO23" s="6"/>
-      <c r="AP23" s="6"/>
+      <c r="AO23" s="25"/>
+      <c r="AP23" s="25"/>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="14"/>
       <c r="AS23" s="16"/>
@@ -2512,7 +2528,7 @@
       <c r="BK23" s="6"/>
       <c r="BL23" s="10"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A24" s="1">
         <v>0.77083333333333304</v>
       </c>
@@ -2580,7 +2596,7 @@
       <c r="BK24" s="6"/>
       <c r="BL24" s="10"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A25" s="1">
         <v>0.79166666666666596</v>
       </c>
@@ -2648,7 +2664,7 @@
       <c r="BK25" s="6"/>
       <c r="BL25" s="10"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.6">
       <c r="A26" s="1">
         <v>0.8125</v>
       </c>
@@ -2716,7 +2732,7 @@
       <c r="BK26" s="6"/>
       <c r="BL26" s="10"/>
     </row>
-    <row r="27" spans="1:64" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A27" s="1">
         <v>0.83333333333333304</v>
       </c>

</xml_diff>

<commit_message>
Adding in my schedule again...
</commit_message>
<xml_diff>
--- a/logistics/planning_for_backlog.xlsx
+++ b/logistics/planning_for_backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\Boise State\Spring 2018\CS471\groupProject\CS471-S18-BitJunkies\logistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\K1ASER\git\CS471-S18-BitJunkies\logistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="15918" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="28800" windowHeight="15924" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deliverables" sheetId="1" r:id="rId1"/>
@@ -141,6 +141,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,13 +159,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,7 +185,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -351,16 +352,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -391,11 +392,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="3" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="3" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="1" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -714,14 +717,14 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30.09765625" customWidth="1"/>
     <col min="3" max="3" width="35.5" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -732,7 +735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>13</v>
       </c>
@@ -740,7 +743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
@@ -748,17 +751,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="7" spans="2:4" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
@@ -766,7 +769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -774,7 +777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -782,7 +785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -799,37 +802,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BL27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" zoomScale="131" workbookViewId="0">
-      <selection activeCell="AP10" sqref="AP10:AP23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="131" workbookViewId="0">
+      <selection activeCell="AY30" sqref="AY30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="7" max="7" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.09765625" customWidth="1"/>
-    <col min="14" max="14" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.09765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.84765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.59765625" customWidth="1"/>
-    <col min="21" max="21" width="3.84765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.796875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="3.09765625" bestFit="1" customWidth="1"/>
     <col min="23" max="64" width="3.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:64" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="23" t="s">
         <v>9</v>
@@ -897,7 +900,7 @@
       <c r="BK1" s="23"/>
       <c r="BL1" s="23"/>
     </row>
-    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:64" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
@@ -962,7 +965,7 @@
       <c r="BK2" s="24"/>
       <c r="BL2" s="24"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1048,7 @@
       <c r="BK3" s="21"/>
       <c r="BL3" s="22"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>0.375</v>
       </c>
@@ -1289,11 +1292,11 @@
       <c r="AV5" s="6"/>
       <c r="AW5" s="6"/>
       <c r="AX5" s="10"/>
-      <c r="AY5" s="9"/>
-      <c r="AZ5" s="6"/>
-      <c r="BA5" s="6"/>
-      <c r="BB5" s="6"/>
-      <c r="BC5" s="6"/>
+      <c r="AY5" s="25"/>
+      <c r="AZ5" s="27"/>
+      <c r="BA5" s="27"/>
+      <c r="BB5" s="27"/>
+      <c r="BC5" s="27"/>
       <c r="BD5" s="6"/>
       <c r="BE5" s="10"/>
       <c r="BF5" s="9"/>
@@ -1304,7 +1307,7 @@
       <c r="BK5" s="6"/>
       <c r="BL5" s="10"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>0.39583333333333331</v>
       </c>
@@ -1357,11 +1360,11 @@
       <c r="AV6" s="6"/>
       <c r="AW6" s="6"/>
       <c r="AX6" s="10"/>
-      <c r="AY6" s="9"/>
-      <c r="AZ6" s="6"/>
-      <c r="BA6" s="6"/>
-      <c r="BB6" s="6"/>
-      <c r="BC6" s="6"/>
+      <c r="AY6" s="25"/>
+      <c r="AZ6" s="27"/>
+      <c r="BA6" s="27"/>
+      <c r="BB6" s="27"/>
+      <c r="BC6" s="27"/>
       <c r="BD6" s="6"/>
       <c r="BE6" s="10"/>
       <c r="BF6" s="9"/>
@@ -1372,7 +1375,7 @@
       <c r="BK6" s="6"/>
       <c r="BL6" s="10"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0.41666666666666702</v>
       </c>
@@ -1425,11 +1428,11 @@
       <c r="AV7" s="6"/>
       <c r="AW7" s="16"/>
       <c r="AX7" s="18"/>
-      <c r="AY7" s="9"/>
-      <c r="AZ7" s="6"/>
-      <c r="BA7" s="6"/>
-      <c r="BB7" s="6"/>
-      <c r="BC7" s="6"/>
+      <c r="AY7" s="25"/>
+      <c r="AZ7" s="27"/>
+      <c r="BA7" s="27"/>
+      <c r="BB7" s="27"/>
+      <c r="BC7" s="27"/>
       <c r="BD7" s="6"/>
       <c r="BE7" s="10"/>
       <c r="BF7" s="9"/>
@@ -1440,7 +1443,7 @@
       <c r="BK7" s="6"/>
       <c r="BL7" s="10"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>0.4375</v>
       </c>
@@ -1493,11 +1496,11 @@
       <c r="AV8" s="6"/>
       <c r="AW8" s="16"/>
       <c r="AX8" s="18"/>
-      <c r="AY8" s="9"/>
-      <c r="AZ8" s="6"/>
-      <c r="BA8" s="6"/>
-      <c r="BB8" s="6"/>
-      <c r="BC8" s="6"/>
+      <c r="AY8" s="25"/>
+      <c r="AZ8" s="27"/>
+      <c r="BA8" s="27"/>
+      <c r="BB8" s="27"/>
+      <c r="BC8" s="27"/>
       <c r="BD8" s="6"/>
       <c r="BE8" s="10"/>
       <c r="BF8" s="9"/>
@@ -1508,7 +1511,7 @@
       <c r="BK8" s="6"/>
       <c r="BL8" s="10"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>0.45833333333333298</v>
       </c>
@@ -1561,11 +1564,11 @@
       <c r="AV9" s="6"/>
       <c r="AW9" s="16"/>
       <c r="AX9" s="18"/>
-      <c r="AY9" s="9"/>
-      <c r="AZ9" s="6"/>
-      <c r="BA9" s="6"/>
-      <c r="BB9" s="6"/>
-      <c r="BC9" s="6"/>
+      <c r="AY9" s="25"/>
+      <c r="AZ9" s="27"/>
+      <c r="BA9" s="27"/>
+      <c r="BB9" s="27"/>
+      <c r="BC9" s="27"/>
       <c r="BD9" s="6"/>
       <c r="BE9" s="10"/>
       <c r="BF9" s="9"/>
@@ -1576,7 +1579,7 @@
       <c r="BK9" s="6"/>
       <c r="BL9" s="10"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>0.47916666666666702</v>
       </c>
@@ -1620,7 +1623,7 @@
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
       <c r="AO10" s="6"/>
-      <c r="AP10" s="25"/>
+      <c r="AP10" s="27"/>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="9"/>
       <c r="AS10" s="6"/>
@@ -1629,11 +1632,11 @@
       <c r="AV10" s="6"/>
       <c r="AW10" s="16"/>
       <c r="AX10" s="18"/>
-      <c r="AY10" s="9"/>
-      <c r="AZ10" s="6"/>
-      <c r="BA10" s="6"/>
-      <c r="BB10" s="6"/>
-      <c r="BC10" s="6"/>
+      <c r="AY10" s="25"/>
+      <c r="AZ10" s="27"/>
+      <c r="BA10" s="27"/>
+      <c r="BB10" s="27"/>
+      <c r="BC10" s="27"/>
       <c r="BD10" s="6"/>
       <c r="BE10" s="10"/>
       <c r="BF10" s="9"/>
@@ -1644,7 +1647,7 @@
       <c r="BK10" s="6"/>
       <c r="BL10" s="10"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>0.5</v>
       </c>
@@ -1688,7 +1691,7 @@
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
       <c r="AO11" s="6"/>
-      <c r="AP11" s="25"/>
+      <c r="AP11" s="27"/>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="9"/>
       <c r="AS11" s="6"/>
@@ -1698,10 +1701,10 @@
       <c r="AW11" s="16"/>
       <c r="AX11" s="18"/>
       <c r="AY11" s="9"/>
-      <c r="AZ11" s="6"/>
+      <c r="AZ11" s="27"/>
       <c r="BA11" s="6"/>
-      <c r="BB11" s="6"/>
-      <c r="BC11" s="6"/>
+      <c r="BB11" s="27"/>
+      <c r="BC11" s="27"/>
       <c r="BD11" s="6"/>
       <c r="BE11" s="10"/>
       <c r="BF11" s="9"/>
@@ -1712,7 +1715,7 @@
       <c r="BK11" s="6"/>
       <c r="BL11" s="10"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>0.52083333333333304</v>
       </c>
@@ -1756,7 +1759,7 @@
       <c r="AM12" s="6"/>
       <c r="AN12" s="6"/>
       <c r="AO12" s="6"/>
-      <c r="AP12" s="25"/>
+      <c r="AP12" s="27"/>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="9"/>
       <c r="AS12" s="6"/>
@@ -1766,10 +1769,10 @@
       <c r="AW12" s="16"/>
       <c r="AX12" s="18"/>
       <c r="AY12" s="9"/>
-      <c r="AZ12" s="6"/>
+      <c r="AZ12" s="27"/>
       <c r="BA12" s="6"/>
-      <c r="BB12" s="6"/>
-      <c r="BC12" s="6"/>
+      <c r="BB12" s="27"/>
+      <c r="BC12" s="27"/>
       <c r="BD12" s="6"/>
       <c r="BE12" s="10"/>
       <c r="BF12" s="9"/>
@@ -1780,7 +1783,7 @@
       <c r="BK12" s="6"/>
       <c r="BL12" s="10"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>0.54166666666666696</v>
       </c>
@@ -1824,7 +1827,7 @@
       <c r="AM13" s="6"/>
       <c r="AN13" s="6"/>
       <c r="AO13" s="6"/>
-      <c r="AP13" s="25"/>
+      <c r="AP13" s="27"/>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="9"/>
       <c r="AS13" s="6"/>
@@ -1834,10 +1837,10 @@
       <c r="AW13" s="16"/>
       <c r="AX13" s="18"/>
       <c r="AY13" s="9"/>
-      <c r="AZ13" s="6"/>
+      <c r="AZ13" s="27"/>
       <c r="BA13" s="6"/>
-      <c r="BB13" s="6"/>
-      <c r="BC13" s="6"/>
+      <c r="BB13" s="27"/>
+      <c r="BC13" s="27"/>
       <c r="BD13" s="6"/>
       <c r="BE13" s="10"/>
       <c r="BF13" s="9"/>
@@ -1848,7 +1851,7 @@
       <c r="BK13" s="6"/>
       <c r="BL13" s="10"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0.5625</v>
       </c>
@@ -1892,7 +1895,7 @@
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
       <c r="AO14" s="6"/>
-      <c r="AP14" s="25"/>
+      <c r="AP14" s="27"/>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="9"/>
       <c r="AS14" s="6"/>
@@ -1902,10 +1905,10 @@
       <c r="AW14" s="16"/>
       <c r="AX14" s="18"/>
       <c r="AY14" s="9"/>
-      <c r="AZ14" s="6"/>
+      <c r="AZ14" s="27"/>
       <c r="BA14" s="6"/>
-      <c r="BB14" s="6"/>
-      <c r="BC14" s="6"/>
+      <c r="BB14" s="27"/>
+      <c r="BC14" s="27"/>
       <c r="BD14" s="6"/>
       <c r="BE14" s="10"/>
       <c r="BF14" s="9"/>
@@ -1916,7 +1919,7 @@
       <c r="BK14" s="6"/>
       <c r="BL14" s="10"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>0.58333333333333304</v>
       </c>
@@ -1955,12 +1958,12 @@
       <c r="AH15" s="6"/>
       <c r="AI15" s="6"/>
       <c r="AJ15" s="10"/>
-      <c r="AK15" s="26"/>
+      <c r="AK15" s="25"/>
       <c r="AL15" s="6"/>
-      <c r="AM15" s="25"/>
+      <c r="AM15" s="27"/>
       <c r="AN15" s="6"/>
-      <c r="AO15" s="25"/>
-      <c r="AP15" s="25"/>
+      <c r="AO15" s="27"/>
+      <c r="AP15" s="27"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="9"/>
       <c r="AS15" s="6"/>
@@ -1970,10 +1973,10 @@
       <c r="AW15" s="16"/>
       <c r="AX15" s="18"/>
       <c r="AY15" s="9"/>
-      <c r="AZ15" s="6"/>
+      <c r="AZ15" s="27"/>
       <c r="BA15" s="6"/>
-      <c r="BB15" s="6"/>
-      <c r="BC15" s="6"/>
+      <c r="BB15" s="27"/>
+      <c r="BC15" s="27"/>
       <c r="BD15" s="6"/>
       <c r="BE15" s="10"/>
       <c r="BF15" s="9"/>
@@ -1984,7 +1987,7 @@
       <c r="BK15" s="6"/>
       <c r="BL15" s="10"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>0.60416666666666596</v>
       </c>
@@ -2023,12 +2026,12 @@
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
       <c r="AJ16" s="10"/>
-      <c r="AK16" s="26"/>
+      <c r="AK16" s="25"/>
       <c r="AL16" s="6"/>
-      <c r="AM16" s="25"/>
+      <c r="AM16" s="27"/>
       <c r="AN16" s="6"/>
-      <c r="AO16" s="25"/>
-      <c r="AP16" s="25"/>
+      <c r="AO16" s="27"/>
+      <c r="AP16" s="27"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="9"/>
       <c r="AS16" s="6"/>
@@ -2038,10 +2041,10 @@
       <c r="AW16" s="16"/>
       <c r="AX16" s="18"/>
       <c r="AY16" s="9"/>
-      <c r="AZ16" s="6"/>
+      <c r="AZ16" s="27"/>
       <c r="BA16" s="6"/>
-      <c r="BB16" s="6"/>
-      <c r="BC16" s="6"/>
+      <c r="BB16" s="27"/>
+      <c r="BC16" s="27"/>
       <c r="BD16" s="6"/>
       <c r="BE16" s="10"/>
       <c r="BF16" s="9"/>
@@ -2052,7 +2055,7 @@
       <c r="BK16" s="6"/>
       <c r="BL16" s="10"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>0.625</v>
       </c>
@@ -2091,25 +2094,25 @@
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
       <c r="AJ17" s="10"/>
-      <c r="AK17" s="26"/>
+      <c r="AK17" s="25"/>
       <c r="AL17" s="6"/>
-      <c r="AM17" s="25"/>
+      <c r="AM17" s="27"/>
       <c r="AN17" s="6"/>
-      <c r="AO17" s="25"/>
-      <c r="AP17" s="25"/>
+      <c r="AO17" s="27"/>
+      <c r="AP17" s="27"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="14"/>
       <c r="AS17" s="6"/>
       <c r="AT17" s="16"/>
       <c r="AU17" s="6"/>
-      <c r="AV17" s="25"/>
+      <c r="AV17" s="27"/>
       <c r="AW17" s="16"/>
       <c r="AX17" s="18"/>
-      <c r="AY17" s="9"/>
-      <c r="AZ17" s="6"/>
-      <c r="BA17" s="6"/>
-      <c r="BB17" s="6"/>
-      <c r="BC17" s="6"/>
+      <c r="AY17" s="25"/>
+      <c r="AZ17" s="27"/>
+      <c r="BA17" s="27"/>
+      <c r="BB17" s="27"/>
+      <c r="BC17" s="27"/>
       <c r="BD17" s="6"/>
       <c r="BE17" s="10"/>
       <c r="BF17" s="9"/>
@@ -2120,7 +2123,7 @@
       <c r="BK17" s="6"/>
       <c r="BL17" s="10"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>0.64583333333333304</v>
       </c>
@@ -2159,12 +2162,12 @@
       <c r="AH18" s="6"/>
       <c r="AI18" s="6"/>
       <c r="AJ18" s="10"/>
-      <c r="AK18" s="26"/>
+      <c r="AK18" s="25"/>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="25"/>
+      <c r="AM18" s="27"/>
       <c r="AN18" s="6"/>
-      <c r="AO18" s="25"/>
-      <c r="AP18" s="25"/>
+      <c r="AO18" s="27"/>
+      <c r="AP18" s="27"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="14"/>
       <c r="AS18" s="6"/>
@@ -2173,11 +2176,11 @@
       <c r="AV18" s="16"/>
       <c r="AW18" s="16"/>
       <c r="AX18" s="18"/>
-      <c r="AY18" s="9"/>
-      <c r="AZ18" s="6"/>
-      <c r="BA18" s="6"/>
-      <c r="BB18" s="6"/>
-      <c r="BC18" s="6"/>
+      <c r="AY18" s="25"/>
+      <c r="AZ18" s="27"/>
+      <c r="BA18" s="27"/>
+      <c r="BB18" s="27"/>
+      <c r="BC18" s="27"/>
       <c r="BD18" s="6"/>
       <c r="BE18" s="10"/>
       <c r="BF18" s="9"/>
@@ -2188,7 +2191,7 @@
       <c r="BK18" s="6"/>
       <c r="BL18" s="10"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>0.66666666666666596</v>
       </c>
@@ -2227,12 +2230,12 @@
       <c r="AH19" s="6"/>
       <c r="AI19" s="6"/>
       <c r="AJ19" s="10"/>
-      <c r="AK19" s="26"/>
+      <c r="AK19" s="25"/>
       <c r="AL19" s="6"/>
-      <c r="AM19" s="25"/>
+      <c r="AM19" s="27"/>
       <c r="AN19" s="6"/>
-      <c r="AO19" s="25"/>
-      <c r="AP19" s="25"/>
+      <c r="AO19" s="27"/>
+      <c r="AP19" s="27"/>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="14"/>
       <c r="AS19" s="6"/>
@@ -2241,11 +2244,11 @@
       <c r="AV19" s="16"/>
       <c r="AW19" s="16"/>
       <c r="AX19" s="18"/>
-      <c r="AY19" s="9"/>
-      <c r="AZ19" s="6"/>
-      <c r="BA19" s="6"/>
-      <c r="BB19" s="6"/>
-      <c r="BC19" s="6"/>
+      <c r="AY19" s="25"/>
+      <c r="AZ19" s="27"/>
+      <c r="BA19" s="27"/>
+      <c r="BB19" s="27"/>
+      <c r="BC19" s="27"/>
       <c r="BD19" s="6"/>
       <c r="BE19" s="10"/>
       <c r="BF19" s="9"/>
@@ -2256,7 +2259,7 @@
       <c r="BK19" s="6"/>
       <c r="BL19" s="10"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>0.6875</v>
       </c>
@@ -2295,12 +2298,12 @@
       <c r="AH20" s="6"/>
       <c r="AI20" s="6"/>
       <c r="AJ20" s="10"/>
-      <c r="AK20" s="26"/>
+      <c r="AK20" s="25"/>
       <c r="AL20" s="6"/>
-      <c r="AM20" s="25"/>
+      <c r="AM20" s="27"/>
       <c r="AN20" s="6"/>
-      <c r="AO20" s="25"/>
-      <c r="AP20" s="25"/>
+      <c r="AO20" s="27"/>
+      <c r="AP20" s="27"/>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="14"/>
       <c r="AS20" s="6"/>
@@ -2309,11 +2312,11 @@
       <c r="AV20" s="16"/>
       <c r="AW20" s="16"/>
       <c r="AX20" s="18"/>
-      <c r="AY20" s="9"/>
-      <c r="AZ20" s="6"/>
-      <c r="BA20" s="6"/>
-      <c r="BB20" s="6"/>
-      <c r="BC20" s="6"/>
+      <c r="AY20" s="25"/>
+      <c r="AZ20" s="27"/>
+      <c r="BA20" s="27"/>
+      <c r="BB20" s="27"/>
+      <c r="BC20" s="27"/>
       <c r="BD20" s="6"/>
       <c r="BE20" s="10"/>
       <c r="BF20" s="9"/>
@@ -2324,7 +2327,7 @@
       <c r="BK20" s="6"/>
       <c r="BL20" s="10"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>0.70833333333333304</v>
       </c>
@@ -2363,12 +2366,12 @@
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
       <c r="AJ21" s="10"/>
-      <c r="AK21" s="26"/>
+      <c r="AK21" s="25"/>
       <c r="AL21" s="6"/>
-      <c r="AM21" s="25"/>
+      <c r="AM21" s="27"/>
       <c r="AN21" s="6"/>
-      <c r="AO21" s="25"/>
-      <c r="AP21" s="25"/>
+      <c r="AO21" s="27"/>
+      <c r="AP21" s="27"/>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="14"/>
       <c r="AS21" s="6"/>
@@ -2377,11 +2380,11 @@
       <c r="AV21" s="16"/>
       <c r="AW21" s="16"/>
       <c r="AX21" s="18"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="6"/>
-      <c r="BA21" s="6"/>
-      <c r="BB21" s="6"/>
-      <c r="BC21" s="6"/>
+      <c r="AY21" s="25"/>
+      <c r="AZ21" s="27"/>
+      <c r="BA21" s="27"/>
+      <c r="BB21" s="27"/>
+      <c r="BC21" s="27"/>
       <c r="BD21" s="6"/>
       <c r="BE21" s="10"/>
       <c r="BF21" s="9"/>
@@ -2392,7 +2395,7 @@
       <c r="BK21" s="6"/>
       <c r="BL21" s="10"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>0.72916666666666596</v>
       </c>
@@ -2431,12 +2434,12 @@
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
       <c r="AJ22" s="10"/>
-      <c r="AK22" s="26"/>
+      <c r="AK22" s="25"/>
       <c r="AL22" s="6"/>
-      <c r="AM22" s="25"/>
+      <c r="AM22" s="27"/>
       <c r="AN22" s="6"/>
-      <c r="AO22" s="25"/>
-      <c r="AP22" s="25"/>
+      <c r="AO22" s="27"/>
+      <c r="AP22" s="27"/>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="14"/>
       <c r="AS22" s="6"/>
@@ -2445,10 +2448,10 @@
       <c r="AV22" s="16"/>
       <c r="AW22" s="16"/>
       <c r="AX22" s="18"/>
-      <c r="AY22" s="9"/>
-      <c r="AZ22" s="6"/>
-      <c r="BA22" s="6"/>
-      <c r="BB22" s="6"/>
+      <c r="AY22" s="25"/>
+      <c r="AZ22" s="27"/>
+      <c r="BA22" s="27"/>
+      <c r="BB22" s="27"/>
       <c r="BC22" s="6"/>
       <c r="BD22" s="6"/>
       <c r="BE22" s="10"/>
@@ -2460,7 +2463,7 @@
       <c r="BK22" s="6"/>
       <c r="BL22" s="10"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>0.75</v>
       </c>
@@ -2499,12 +2502,12 @@
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
       <c r="AJ23" s="10"/>
-      <c r="AK23" s="26"/>
+      <c r="AK23" s="25"/>
       <c r="AL23" s="6"/>
-      <c r="AM23" s="25"/>
+      <c r="AM23" s="27"/>
       <c r="AN23" s="6"/>
-      <c r="AO23" s="25"/>
-      <c r="AP23" s="25"/>
+      <c r="AO23" s="27"/>
+      <c r="AP23" s="27"/>
       <c r="AQ23" s="10"/>
       <c r="AR23" s="14"/>
       <c r="AS23" s="16"/>
@@ -2513,10 +2516,10 @@
       <c r="AV23" s="16"/>
       <c r="AW23" s="16"/>
       <c r="AX23" s="18"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="6"/>
-      <c r="BA23" s="6"/>
-      <c r="BB23" s="6"/>
+      <c r="AY23" s="25"/>
+      <c r="AZ23" s="27"/>
+      <c r="BA23" s="27"/>
+      <c r="BB23" s="27"/>
       <c r="BC23" s="6"/>
       <c r="BD23" s="6"/>
       <c r="BE23" s="10"/>
@@ -2528,7 +2531,7 @@
       <c r="BK23" s="6"/>
       <c r="BL23" s="10"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>0.77083333333333304</v>
       </c>
@@ -2581,10 +2584,10 @@
       <c r="AV24" s="16"/>
       <c r="AW24" s="16"/>
       <c r="AX24" s="18"/>
-      <c r="AY24" s="9"/>
-      <c r="AZ24" s="6"/>
-      <c r="BA24" s="6"/>
-      <c r="BB24" s="6"/>
+      <c r="AY24" s="25"/>
+      <c r="AZ24" s="27"/>
+      <c r="BA24" s="27"/>
+      <c r="BB24" s="27"/>
       <c r="BC24" s="6"/>
       <c r="BD24" s="6"/>
       <c r="BE24" s="10"/>
@@ -2596,7 +2599,7 @@
       <c r="BK24" s="6"/>
       <c r="BL24" s="10"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.79166666666666596</v>
       </c>
@@ -2649,10 +2652,10 @@
       <c r="AV25" s="16"/>
       <c r="AW25" s="16"/>
       <c r="AX25" s="10"/>
-      <c r="AY25" s="9"/>
-      <c r="AZ25" s="6"/>
-      <c r="BA25" s="6"/>
-      <c r="BB25" s="6"/>
+      <c r="AY25" s="25"/>
+      <c r="AZ25" s="27"/>
+      <c r="BA25" s="27"/>
+      <c r="BB25" s="27"/>
       <c r="BC25" s="6"/>
       <c r="BD25" s="6"/>
       <c r="BE25" s="10"/>
@@ -2664,7 +2667,7 @@
       <c r="BK25" s="6"/>
       <c r="BL25" s="10"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>0.8125</v>
       </c>
@@ -2717,10 +2720,10 @@
       <c r="AV26" s="16"/>
       <c r="AW26" s="16"/>
       <c r="AX26" s="10"/>
-      <c r="AY26" s="9"/>
-      <c r="AZ26" s="6"/>
-      <c r="BA26" s="6"/>
-      <c r="BB26" s="6"/>
+      <c r="AY26" s="25"/>
+      <c r="AZ26" s="27"/>
+      <c r="BA26" s="27"/>
+      <c r="BB26" s="27"/>
       <c r="BC26" s="6"/>
       <c r="BD26" s="6"/>
       <c r="BE26" s="10"/>
@@ -2732,7 +2735,7 @@
       <c r="BK26" s="6"/>
       <c r="BL26" s="10"/>
     </row>
-    <row r="27" spans="1:64" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:64" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>0.83333333333333304</v>
       </c>
@@ -2785,10 +2788,10 @@
       <c r="AV27" s="17"/>
       <c r="AW27" s="17"/>
       <c r="AX27" s="13"/>
-      <c r="AY27" s="11"/>
-      <c r="AZ27" s="12"/>
-      <c r="BA27" s="12"/>
-      <c r="BB27" s="12"/>
+      <c r="AY27" s="26"/>
+      <c r="AZ27" s="28"/>
+      <c r="BA27" s="28"/>
+      <c r="BB27" s="28"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
       <c r="BE27" s="13"/>

</xml_diff>